<commit_message>
Hoang add ReportManagement, UserManagement include entity, controller, dao, service, serviceimpl, jsp
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="0 3 2024" r:id="rId3" sheetId="1"/>
+    <sheet name="2 2 2024" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>#</t>
   </si>
@@ -26,10 +26,7 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>2024-03-02T00:00</t>
-  </si>
-  <si>
-    <t>2024-03-03T00:00</t>
+    <t>2023-02-02T00:00</t>
   </si>
 </sst>
 </file>
@@ -74,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,20 +105,6 @@
         <v>1500.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>500.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Duy Anh - Thêm Đa ngôn ngữ
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2 2 2024" r:id="rId3" sheetId="1"/>
+    <sheet name="201124" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -26,7 +26,7 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>2023-02-02T00:00</t>
+    <t>2024-02-03T14:56:59.270677</t>
   </si>
 </sst>
 </file>
@@ -99,10 +99,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1500.0</v>
+        <v>78000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoang add spring security login with google, modify columnDefinition firstName, lastName of User, add home() at UserController, add findByUsername() add UserService, UserServiceImpl, edit application.properties, edit pom.xml
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="201124" r:id="rId3" sheetId="1"/>
+    <sheet name="2 0 0" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>#</t>
   </si>
@@ -26,7 +26,13 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>2024-02-03T14:56:59.270677</t>
+    <t>2023-02-02T00:00</t>
+  </si>
+  <si>
+    <t>2024-03-02T00:00</t>
+  </si>
+  <si>
+    <t>2024-02-02T00:00</t>
   </si>
 </sst>
 </file>
@@ -71,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,10 +105,38 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1.0</v>
       </c>
-      <c r="D2" t="n">
-        <v>78000.0</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy Anh test pull x1
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="201124" r:id="rId3" sheetId="1"/>
+    <sheet name="221124" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -24,6 +24,21 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>2024-02-20T19:12:57.649412</t>
+  </si>
+  <si>
+    <t>2024-02-20T19:15:24.768470</t>
+  </si>
+  <si>
+    <t>2024-02-21T15:29:24.108602</t>
+  </si>
+  <si>
+    <t>2024-02-21T15:29:45.516237</t>
+  </si>
+  <si>
+    <t>2024-02-21T18:10:47.988877</t>
   </si>
   <si>
     <t>2024-02-03T14:56:59.270677</t>
@@ -71,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,6 +117,76 @@
         <v>1.0</v>
       </c>
       <c r="D2" t="n">
+        <v>107000.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>107000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>107000.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>107000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>107000.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D7" t="n">
         <v>78000.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nguyen da cap nhat 22/02
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -26,7 +26,7 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>2024-02-03T14:56:59.270677</t>
+    <t>2024-02-20T19:15:07.827588</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,7 @@
         <v>1.0</v>
       </c>
       <c r="D2" t="n">
-        <v>78000.0</v>
+        <v>39000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>